<commit_message>
One more year of data.
</commit_message>
<xml_diff>
--- a/drugs/medicine.xlsx
+++ b/drugs/medicine.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\lucent\health-data\drugs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E623D956-4AAC-4998-B84B-DBFF8BA44F3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0CCFA89-F2B1-465A-8D9B-23775E24F6DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1905" yWindow="1800" windowWidth="28140" windowHeight="19425" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8010" yWindow="870" windowWidth="30375" windowHeight="20505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="51">
   <si>
     <t>Date</t>
   </si>
@@ -55,19 +55,149 @@
   </si>
   <si>
     <t>Lot</t>
+  </si>
+  <si>
+    <t>R R Stomach</t>
+  </si>
+  <si>
+    <t>Expiry</t>
+  </si>
+  <si>
+    <t>D735992D</t>
+  </si>
+  <si>
+    <t>Subjective strength</t>
+  </si>
+  <si>
+    <t>low</t>
+  </si>
+  <si>
+    <t>high</t>
+  </si>
+  <si>
+    <t>very low</t>
+  </si>
+  <si>
+    <t>Serial</t>
+  </si>
+  <si>
+    <t>D746439A</t>
+  </si>
+  <si>
+    <t>369574751668</t>
+  </si>
+  <si>
+    <t>309736030503</t>
+  </si>
+  <si>
+    <t>R T Stomach</t>
+  </si>
+  <si>
+    <t>L L Stomach</t>
+  </si>
+  <si>
+    <t>L T Stomach</t>
+  </si>
+  <si>
+    <t>very high</t>
+  </si>
+  <si>
+    <t>R L Stomach</t>
+  </si>
+  <si>
+    <t>D736216D</t>
+  </si>
+  <si>
+    <t>313084754648</t>
+  </si>
+  <si>
+    <t>D738490D</t>
+  </si>
+  <si>
+    <t>323563906677</t>
+  </si>
+  <si>
+    <t>L UU Stomach</t>
+  </si>
+  <si>
+    <t>L Thigh</t>
+  </si>
+  <si>
+    <t>delayed onset</t>
+  </si>
+  <si>
+    <t>349319171777</t>
+  </si>
+  <si>
+    <t>D790193A</t>
+  </si>
+  <si>
+    <t>321179678092</t>
+  </si>
+  <si>
+    <t>medium</t>
+  </si>
+  <si>
+    <t>D772233C</t>
+  </si>
+  <si>
+    <t>388462861905</t>
+  </si>
+  <si>
+    <t>D793672D</t>
+  </si>
+  <si>
+    <t>096594151986</t>
+  </si>
+  <si>
+    <t>metformin XR 500</t>
+  </si>
+  <si>
+    <t>high start low end</t>
+  </si>
+  <si>
+    <t>D814653D</t>
+  </si>
+  <si>
+    <t>388082724768</t>
+  </si>
+  <si>
+    <t>095399808123</t>
+  </si>
+  <si>
+    <t>M Stomach</t>
+  </si>
+  <si>
+    <t>D863001A</t>
+  </si>
+  <si>
+    <t>351794997754</t>
+  </si>
+  <si>
+    <t>D837896D</t>
+  </si>
+  <si>
+    <t>383877302654</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="[$-409]m/d/yy\ h:mm\ AM/PM;@"/>
+    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -93,9 +223,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -376,20 +508,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:H52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -405,8 +542,17 @@
       <c r="E1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>45552.541666666664</v>
       </c>
@@ -419,8 +565,20 @@
       <c r="D2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" s="3">
+        <v>46102</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>45559.5</v>
       </c>
@@ -433,8 +591,20 @@
       <c r="D3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" s="3">
+        <v>46102</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>45566.5</v>
       </c>
@@ -447,8 +617,20 @@
       <c r="D4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" s="3">
+        <v>46102</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>45573.5</v>
       </c>
@@ -461,8 +643,1114 @@
       <c r="D5" t="s">
         <v>8</v>
       </c>
+      <c r="E5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" s="3">
+        <v>46102</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>45580.5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6">
+        <v>5</v>
+      </c>
+      <c r="D6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" s="3">
+        <v>46141</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>45587.5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7">
+        <v>5</v>
+      </c>
+      <c r="D7" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" s="3">
+        <v>46141</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>45594.583333333336</v>
+      </c>
+      <c r="B8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C8">
+        <v>5</v>
+      </c>
+      <c r="D8" t="s">
+        <v>21</v>
+      </c>
+      <c r="E8" t="s">
+        <v>12</v>
+      </c>
+      <c r="F8" s="3">
+        <v>46141</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>45601.5</v>
+      </c>
+      <c r="B9" t="s">
+        <v>2</v>
+      </c>
+      <c r="C9">
+        <v>5</v>
+      </c>
+      <c r="D9" t="s">
+        <v>23</v>
+      </c>
+      <c r="E9" t="s">
+        <v>12</v>
+      </c>
+      <c r="F9" s="3">
+        <v>46141</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>45608.5</v>
+      </c>
+      <c r="B10" t="s">
+        <v>2</v>
+      </c>
+      <c r="C10">
+        <v>5</v>
+      </c>
+      <c r="D10" t="s">
+        <v>25</v>
+      </c>
+      <c r="E10" t="s">
+        <v>26</v>
+      </c>
+      <c r="F10" s="3">
+        <v>46139</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>45615.5</v>
+      </c>
+      <c r="B11" t="s">
+        <v>2</v>
+      </c>
+      <c r="C11">
+        <v>5</v>
+      </c>
+      <c r="E11" t="s">
+        <v>26</v>
+      </c>
+      <c r="F11" s="3">
+        <v>46139</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>45622.5</v>
+      </c>
+      <c r="B12" t="s">
+        <v>2</v>
+      </c>
+      <c r="C12">
+        <v>5</v>
+      </c>
+      <c r="E12" t="s">
+        <v>26</v>
+      </c>
+      <c r="F12" s="3">
+        <v>46139</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>45629.5</v>
+      </c>
+      <c r="B13" t="s">
+        <v>2</v>
+      </c>
+      <c r="C13">
+        <v>5</v>
+      </c>
+      <c r="E13" t="s">
+        <v>26</v>
+      </c>
+      <c r="F13" s="3">
+        <v>46139</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>45636.75</v>
+      </c>
+      <c r="B14" t="s">
+        <v>2</v>
+      </c>
+      <c r="C14">
+        <v>5</v>
+      </c>
+      <c r="D14" t="s">
+        <v>30</v>
+      </c>
+      <c r="E14" t="s">
+        <v>28</v>
+      </c>
+      <c r="F14" s="3">
+        <v>46154</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>45645.5</v>
+      </c>
+      <c r="B15" t="s">
+        <v>2</v>
+      </c>
+      <c r="C15">
+        <v>5</v>
+      </c>
+      <c r="D15" t="s">
+        <v>31</v>
+      </c>
+      <c r="E15" t="s">
+        <v>28</v>
+      </c>
+      <c r="F15" s="3">
+        <v>46154</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H15" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>45650.583333333336</v>
+      </c>
+      <c r="B16" t="s">
+        <v>2</v>
+      </c>
+      <c r="C16">
+        <v>5</v>
+      </c>
+      <c r="D16" t="s">
+        <v>21</v>
+      </c>
+      <c r="E16" t="s">
+        <v>28</v>
+      </c>
+      <c r="F16" s="3">
+        <v>46154</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H16" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>45657.5</v>
+      </c>
+      <c r="B17" t="s">
+        <v>2</v>
+      </c>
+      <c r="C17">
+        <v>5</v>
+      </c>
+      <c r="D17" t="s">
+        <v>23</v>
+      </c>
+      <c r="E17" t="s">
+        <v>28</v>
+      </c>
+      <c r="F17" s="3">
+        <v>46154</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H17" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>45664.541666666664</v>
+      </c>
+      <c r="B18" t="s">
+        <v>2</v>
+      </c>
+      <c r="C18">
+        <v>5</v>
+      </c>
+      <c r="D18" t="s">
+        <v>21</v>
+      </c>
+      <c r="E18" t="s">
+        <v>28</v>
+      </c>
+      <c r="F18" s="3">
+        <v>46154</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="H18" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>45671.625</v>
+      </c>
+      <c r="B19" t="s">
+        <v>2</v>
+      </c>
+      <c r="C19">
+        <v>5</v>
+      </c>
+      <c r="D19" t="s">
+        <v>5</v>
+      </c>
+      <c r="E19" t="s">
+        <v>28</v>
+      </c>
+      <c r="F19" s="3">
+        <v>46154</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="H19" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>45678.645833333336</v>
+      </c>
+      <c r="B20" t="s">
+        <v>2</v>
+      </c>
+      <c r="C20">
+        <v>5</v>
+      </c>
+      <c r="D20" t="s">
+        <v>6</v>
+      </c>
+      <c r="E20" t="s">
+        <v>28</v>
+      </c>
+      <c r="F20" s="3">
+        <v>46154</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>45685.541666666664</v>
+      </c>
+      <c r="B21" t="s">
+        <v>2</v>
+      </c>
+      <c r="C21">
+        <v>5</v>
+      </c>
+      <c r="D21" t="s">
+        <v>5</v>
+      </c>
+      <c r="E21" t="s">
+        <v>28</v>
+      </c>
+      <c r="F21" s="3">
+        <v>46154</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>45692.604166666664</v>
+      </c>
+      <c r="B22" t="s">
+        <v>2</v>
+      </c>
+      <c r="C22">
+        <v>5</v>
+      </c>
+      <c r="D22" t="s">
+        <v>6</v>
+      </c>
+      <c r="E22" t="s">
+        <v>34</v>
+      </c>
+      <c r="F22" s="3">
+        <v>46178</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>45699.5625</v>
+      </c>
+      <c r="B23" t="s">
+        <v>2</v>
+      </c>
+      <c r="C23">
+        <v>5</v>
+      </c>
+      <c r="D23" t="s">
+        <v>5</v>
+      </c>
+      <c r="E23" t="s">
+        <v>34</v>
+      </c>
+      <c r="F23" s="3">
+        <v>46178</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="H23" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <v>45706.625</v>
+      </c>
+      <c r="B24" t="s">
+        <v>2</v>
+      </c>
+      <c r="C24">
+        <v>5</v>
+      </c>
+      <c r="D24" t="s">
+        <v>6</v>
+      </c>
+      <c r="E24" t="s">
+        <v>34</v>
+      </c>
+      <c r="F24" s="3">
+        <v>46178</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="H24" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
+        <v>45713.625</v>
+      </c>
+      <c r="B25" t="s">
+        <v>2</v>
+      </c>
+      <c r="C25">
+        <v>5</v>
+      </c>
+      <c r="D25" t="s">
+        <v>5</v>
+      </c>
+      <c r="E25" t="s">
+        <v>34</v>
+      </c>
+      <c r="F25" s="3">
+        <v>46178</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="H25" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
+        <v>45720.583333333336</v>
+      </c>
+      <c r="B26" t="s">
+        <v>2</v>
+      </c>
+      <c r="C26">
+        <v>7.5</v>
+      </c>
+      <c r="D26" t="s">
+        <v>6</v>
+      </c>
+      <c r="E26" t="s">
+        <v>37</v>
+      </c>
+      <c r="F26" s="3">
+        <v>46258</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="H26" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
+        <v>45727.645833333336</v>
+      </c>
+      <c r="B27" t="s">
+        <v>2</v>
+      </c>
+      <c r="C27">
+        <v>7.5</v>
+      </c>
+      <c r="D27" t="s">
+        <v>5</v>
+      </c>
+      <c r="E27" t="s">
+        <v>37</v>
+      </c>
+      <c r="F27" s="3">
+        <v>46258</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="H27" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
+        <v>45734.645833333336</v>
+      </c>
+      <c r="B28" t="s">
+        <v>2</v>
+      </c>
+      <c r="C28">
+        <v>7.5</v>
+      </c>
+      <c r="D28" t="s">
+        <v>6</v>
+      </c>
+      <c r="E28" t="s">
+        <v>37</v>
+      </c>
+      <c r="F28" s="3">
+        <v>46258</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="H28" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="1">
+        <v>45741.583333333336</v>
+      </c>
+      <c r="B29" t="s">
+        <v>2</v>
+      </c>
+      <c r="C29">
+        <v>7.5</v>
+      </c>
+      <c r="D29" t="s">
+        <v>5</v>
+      </c>
+      <c r="E29" t="s">
+        <v>37</v>
+      </c>
+      <c r="F29" s="3">
+        <v>46258</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="H29" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
+        <v>45748.666666666664</v>
+      </c>
+      <c r="B30" t="s">
+        <v>2</v>
+      </c>
+      <c r="C30">
+        <v>7.5</v>
+      </c>
+      <c r="D30" t="s">
+        <v>6</v>
+      </c>
+      <c r="E30" t="s">
+        <v>39</v>
+      </c>
+      <c r="F30" s="3">
+        <v>46317</v>
+      </c>
+      <c r="G30" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="H30" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" s="1">
+        <v>45755.8125</v>
+      </c>
+      <c r="B31" t="s">
+        <v>2</v>
+      </c>
+      <c r="C31">
+        <v>7.5</v>
+      </c>
+      <c r="D31" t="s">
+        <v>5</v>
+      </c>
+      <c r="E31" t="s">
+        <v>39</v>
+      </c>
+      <c r="F31" s="3">
+        <v>46317</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="H31" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" s="1">
+        <v>45762.645833333336</v>
+      </c>
+      <c r="B32" t="s">
+        <v>2</v>
+      </c>
+      <c r="C32">
+        <v>7.5</v>
+      </c>
+      <c r="D32" t="s">
+        <v>6</v>
+      </c>
+      <c r="E32" t="s">
+        <v>39</v>
+      </c>
+      <c r="F32" s="3">
+        <v>46317</v>
+      </c>
+      <c r="G32" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="H32" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" s="1">
+        <v>45769.666666666664</v>
+      </c>
+      <c r="B33" t="s">
+        <v>2</v>
+      </c>
+      <c r="C33">
+        <v>7.5</v>
+      </c>
+      <c r="D33" t="s">
+        <v>5</v>
+      </c>
+      <c r="E33" t="s">
+        <v>39</v>
+      </c>
+      <c r="F33" s="3">
+        <v>46317</v>
+      </c>
+      <c r="G33" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="H33" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34" s="1">
+        <v>45776.666666666664</v>
+      </c>
+      <c r="B34" t="s">
+        <v>2</v>
+      </c>
+      <c r="C34">
+        <v>7.5</v>
+      </c>
+      <c r="D34" t="s">
+        <v>6</v>
+      </c>
+      <c r="E34" t="s">
+        <v>39</v>
+      </c>
+      <c r="F34" s="3">
+        <v>46317</v>
+      </c>
+      <c r="G34" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="H34" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35" s="1">
+        <v>45783.708333333336</v>
+      </c>
+      <c r="B35" t="s">
+        <v>2</v>
+      </c>
+      <c r="C35">
+        <v>7.5</v>
+      </c>
+      <c r="D35" t="s">
+        <v>5</v>
+      </c>
+      <c r="E35" t="s">
+        <v>39</v>
+      </c>
+      <c r="F35" s="3">
+        <v>46317</v>
+      </c>
+      <c r="G35" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="H35" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36" s="1">
+        <v>45790.666666666664</v>
+      </c>
+      <c r="B36" t="s">
+        <v>2</v>
+      </c>
+      <c r="C36">
+        <v>7.5</v>
+      </c>
+      <c r="D36" t="s">
+        <v>6</v>
+      </c>
+      <c r="E36" t="s">
+        <v>39</v>
+      </c>
+      <c r="F36" s="3">
+        <v>46317</v>
+      </c>
+      <c r="G36" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37" s="1">
+        <v>45797.624999884261</v>
+      </c>
+      <c r="B37" t="s">
+        <v>2</v>
+      </c>
+      <c r="C37">
+        <v>7.5</v>
+      </c>
+      <c r="D37" t="s">
+        <v>5</v>
+      </c>
+      <c r="E37" t="s">
+        <v>39</v>
+      </c>
+      <c r="F37" s="3">
+        <v>46317</v>
+      </c>
+      <c r="G37" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A38" s="1">
+        <v>45804.666666666664</v>
+      </c>
+      <c r="B38" t="s">
+        <v>2</v>
+      </c>
+      <c r="C38">
+        <v>10</v>
+      </c>
+      <c r="D38" t="s">
+        <v>6</v>
+      </c>
+      <c r="E38" t="s">
+        <v>43</v>
+      </c>
+      <c r="F38" s="3">
+        <v>46385</v>
+      </c>
+      <c r="G38" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39" s="1">
+        <v>45811.625</v>
+      </c>
+      <c r="B39" t="s">
+        <v>2</v>
+      </c>
+      <c r="C39">
+        <v>10</v>
+      </c>
+      <c r="D39" t="s">
+        <v>5</v>
+      </c>
+      <c r="E39" t="s">
+        <v>43</v>
+      </c>
+      <c r="F39" s="3">
+        <v>46385</v>
+      </c>
+      <c r="G39" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40" s="1">
+        <v>45818.625</v>
+      </c>
+      <c r="B40" t="s">
+        <v>2</v>
+      </c>
+      <c r="C40">
+        <v>10</v>
+      </c>
+      <c r="D40" t="s">
+        <v>6</v>
+      </c>
+      <c r="E40" t="s">
+        <v>43</v>
+      </c>
+      <c r="F40" s="3">
+        <v>46385</v>
+      </c>
+      <c r="G40" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41" s="1">
+        <v>45825.666666666664</v>
+      </c>
+      <c r="B41" t="s">
+        <v>2</v>
+      </c>
+      <c r="C41">
+        <v>10</v>
+      </c>
+      <c r="D41" t="s">
+        <v>5</v>
+      </c>
+      <c r="E41" t="s">
+        <v>43</v>
+      </c>
+      <c r="F41" s="3">
+        <v>46385</v>
+      </c>
+      <c r="G41" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A42" s="1">
+        <v>45832.70833321759</v>
+      </c>
+      <c r="B42" t="s">
+        <v>2</v>
+      </c>
+      <c r="C42">
+        <v>10</v>
+      </c>
+      <c r="D42" t="s">
+        <v>6</v>
+      </c>
+      <c r="E42" t="s">
+        <v>47</v>
+      </c>
+      <c r="F42" s="3">
+        <v>46317</v>
+      </c>
+      <c r="G42" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A43" s="1">
+        <v>45839.666666666664</v>
+      </c>
+      <c r="B43" t="s">
+        <v>2</v>
+      </c>
+      <c r="C43">
+        <v>10</v>
+      </c>
+      <c r="D43" t="s">
+        <v>5</v>
+      </c>
+      <c r="E43" t="s">
+        <v>47</v>
+      </c>
+      <c r="F43" s="3">
+        <v>46317</v>
+      </c>
+      <c r="G43" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A44" s="1">
+        <v>45846.708333333336</v>
+      </c>
+      <c r="B44" t="s">
+        <v>2</v>
+      </c>
+      <c r="C44">
+        <v>10</v>
+      </c>
+      <c r="D44" t="s">
+        <v>6</v>
+      </c>
+      <c r="E44" t="s">
+        <v>47</v>
+      </c>
+      <c r="F44" s="3">
+        <v>46317</v>
+      </c>
+      <c r="G44" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A45" s="1">
+        <v>45853.999305555553</v>
+      </c>
+      <c r="B45" t="s">
+        <v>2</v>
+      </c>
+      <c r="C45">
+        <v>10</v>
+      </c>
+      <c r="D45" t="s">
+        <v>46</v>
+      </c>
+      <c r="E45" t="s">
+        <v>47</v>
+      </c>
+      <c r="F45" s="3">
+        <v>46317</v>
+      </c>
+      <c r="G45" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A46" s="1">
+        <v>45860.708333333336</v>
+      </c>
+      <c r="B46" t="s">
+        <v>2</v>
+      </c>
+      <c r="C46">
+        <v>10</v>
+      </c>
+      <c r="D46" t="s">
+        <v>5</v>
+      </c>
+      <c r="E46" t="s">
+        <v>49</v>
+      </c>
+      <c r="F46" s="3">
+        <v>46457</v>
+      </c>
+      <c r="G46" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A47" s="1">
+        <v>45867.8125</v>
+      </c>
+      <c r="B47" t="s">
+        <v>2</v>
+      </c>
+      <c r="C47">
+        <v>10</v>
+      </c>
+      <c r="D47" t="s">
+        <v>6</v>
+      </c>
+      <c r="E47" t="s">
+        <v>49</v>
+      </c>
+      <c r="F47" s="3">
+        <v>46457</v>
+      </c>
+      <c r="G47" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A48" s="1">
+        <v>45874.770833333336</v>
+      </c>
+      <c r="B48" t="s">
+        <v>2</v>
+      </c>
+      <c r="C48">
+        <v>10</v>
+      </c>
+      <c r="D48" t="s">
+        <v>5</v>
+      </c>
+      <c r="E48" t="s">
+        <v>49</v>
+      </c>
+      <c r="F48" s="3">
+        <v>46457</v>
+      </c>
+      <c r="G48" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A49" s="1">
+        <v>45881.708333333336</v>
+      </c>
+      <c r="B49" t="s">
+        <v>2</v>
+      </c>
+      <c r="C49">
+        <v>10</v>
+      </c>
+      <c r="D49" t="s">
+        <v>6</v>
+      </c>
+      <c r="E49" t="s">
+        <v>49</v>
+      </c>
+      <c r="F49" s="3">
+        <v>46457</v>
+      </c>
+      <c r="G49" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A50" s="1">
+        <v>45747.5</v>
+      </c>
+      <c r="B50" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A51" s="1">
+        <v>45748.5</v>
+      </c>
+      <c r="B51" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A52" s="1">
+        <v>45748.875</v>
+      </c>
+      <c r="B52" t="s">
+        <v>41</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>